<commit_message>
-Correcting some documentaion issues
</commit_message>
<xml_diff>
--- a/H01R02/Released/BOM/H01R02.xlsx
+++ b/H01R02/Released/BOM/H01R02.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Obada\Desktop\hex\My Design\Led\H01R0x-Hardware-Stm32-G0\H01R02\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\OneDrive\Documents\H01R0x-Hardware\H01R02\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD6F67C-4591-4E6C-B1E2-F109EE0199AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H21R00" sheetId="1" r:id="rId1"/>
+    <sheet name="H01R02" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -318,7 +319,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -501,23 +502,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,13 +516,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -548,7 +532,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -565,27 +548,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -606,6 +568,54 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,468 +991,467 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.5546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.33203125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="46.2" x14ac:dyDescent="0.85">
+      <c r="A2" s="7"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="16">
         <v>2</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="17">
         <v>44739</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:9" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:9" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="34">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="34">
         <v>1</v>
       </c>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+    </row>
+    <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    <row r="20" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:6" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+    <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="34">
         <v>1</v>
       </c>
     </row>
@@ -1453,22 +1462,22 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1"/>
-    <hyperlink ref="E21" r:id="rId2"/>
-    <hyperlink ref="E12" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="E15" r:id="rId5"/>
-    <hyperlink ref="E16" r:id="rId6"/>
-    <hyperlink ref="E20" r:id="rId7"/>
-    <hyperlink ref="E22" r:id="rId8"/>
-    <hyperlink ref="E23" r:id="rId9"/>
-    <hyperlink ref="E25" r:id="rId10"/>
-    <hyperlink ref="E14" r:id="rId11"/>
-    <hyperlink ref="E17" r:id="rId12"/>
-    <hyperlink ref="C24" r:id="rId13" display="https://octopart.com/manufacturers/wolfspeed"/>
-    <hyperlink ref="E10" r:id="rId14"/>
-    <hyperlink ref="E18" r:id="rId15"/>
-    <hyperlink ref="E19" r:id="rId16"/>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E23" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E25" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C24" r:id="rId13" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>

</xml_diff>